<commit_message>
grafico ram e lvl1, incompleto
</commit_message>
<xml_diff>
--- a/gráficos.xlsx
+++ b/gráficos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="714" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="714"/>
   </bookViews>
   <sheets>
     <sheet name="19KBytes-641" sheetId="6" r:id="rId1"/>
@@ -251,7 +251,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="96">
+  <cellStyleXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -348,6 +348,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -413,7 +417,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="96">
+  <cellStyles count="100">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -461,6 +465,8 @@
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -508,6 +514,8 @@
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="79"/>
   </cellStyles>
@@ -600,29 +608,26 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -630,29 +635,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$K$6:$K$12</c:f>
+              <c:f>'19KBytes-641'!$K$6:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.009965</c:v>
+                  <c:v>0.009834</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.009834</c:v>
+                  <c:v>0.014631</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.014631</c:v>
+                  <c:v>0.017262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.017262</c:v>
+                  <c:v>0.019785</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.019785</c:v>
+                  <c:v>0.026098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.026098</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.03125</c:v>
                 </c:pt>
               </c:numCache>
@@ -664,7 +666,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:ln w="38100" cmpd="sng">
+            <a:ln>
               <a:prstDash val="sysDot"/>
             </a:ln>
           </c:spPr>
@@ -676,29 +678,26 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -706,30 +705,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$M$6:$M$12</c:f>
+              <c:f>'19KBytes-641'!$M$6:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.009965</c:v>
+                  <c:v>0.009834</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0049825</c:v>
+                  <c:v>0.004917</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00249125</c:v>
+                  <c:v>0.0024585</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.001245625</c:v>
+                  <c:v>0.00122925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0006228125</c:v>
+                  <c:v>0.0008195</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.000415208333333333</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.00031140625</c:v>
+                  <c:v>0.000614625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,11 +743,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2118750584"/>
-        <c:axId val="2109121736"/>
+        <c:axId val="2094434776"/>
+        <c:axId val="2094442408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2118750584"/>
+        <c:axId val="2094434776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -778,13 +774,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>N</a:t>
+                  <a:t>Número de processos</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>úmero de processos</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -842,7 +833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109121736"/>
+        <c:crossAx val="2094442408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -850,7 +841,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109121736"/>
+        <c:axId val="2094442408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,7 +935,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118750584"/>
+        <c:crossAx val="2094434776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1069,29 +1060,26 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1099,30 +1087,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$N$6:$N$12</c:f>
+              <c:f>'19KBytes-641'!$N$6:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.013321130770795</c:v>
+                  <c:v>0.672134508919418</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.681088100608297</c:v>
+                  <c:v>0.569690649982621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.577279573629939</c:v>
+                  <c:v>0.497043214556482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.503664392216326</c:v>
+                  <c:v>0.376810483561959</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.381830025289294</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.31888</c:v>
+                  <c:v>0.314688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1149,29 +1134,26 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1211,11 +1193,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2134803656"/>
-        <c:axId val="-2138606440"/>
+        <c:axId val="2094516184"/>
+        <c:axId val="2094522584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2134803656"/>
+        <c:axId val="2094516184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,11 +1224,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>N</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>úmero de processos</a:t>
+                  <a:t>Número de processos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1305,7 +1283,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138606440"/>
+        <c:crossAx val="2094522584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1313,7 +1291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138606440"/>
+        <c:axId val="2094522584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,7 +1385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134803656"/>
+        <c:crossAx val="2094516184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1528,29 +1506,26 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:f>'19KBytes-662'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1558,30 +1533,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$M$6:$M$12</c:f>
+              <c:f>'19KBytes-662'!$M$6:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.009965</c:v>
+                  <c:v>0.011055</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0049825</c:v>
+                  <c:v>0.0055275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00249125</c:v>
+                  <c:v>0.00276375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.001245625</c:v>
+                  <c:v>0.001381875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0006228125</c:v>
+                  <c:v>0.00092125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.000415208333333333</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.00031140625</c:v>
+                  <c:v>0.0006909375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1589,8 +1561,17 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1599,29 +1580,26 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:f>'19KBytes-662'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1629,29 +1607,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-662'!$K$6:$K$12</c:f>
+              <c:f>'19KBytes-662'!$K$6:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.009965</c:v>
+                  <c:v>0.011055</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.011055</c:v>
+                  <c:v>0.01671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.01671</c:v>
+                  <c:v>0.019255</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.019255</c:v>
+                  <c:v>0.023469</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.023469</c:v>
+                  <c:v>0.026969</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.026969</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.033032</c:v>
                 </c:pt>
               </c:numCache>
@@ -1670,11 +1645,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2062614536"/>
-        <c:axId val="2063474904"/>
+        <c:axId val="2093408520"/>
+        <c:axId val="2093414936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2062614536"/>
+        <c:axId val="2093408520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,13 +1676,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>N</a:t>
+                  <a:t>Número de processos</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>úmero de processos</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1765,7 +1735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2063474904"/>
+        <c:crossAx val="2093414936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1773,7 +1743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2063474904"/>
+        <c:axId val="2093414936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +1837,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2062614536"/>
+        <c:crossAx val="2093408520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1992,29 +1962,26 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2022,30 +1989,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$N$6:$N$12</c:f>
+              <c:f>'19KBytes-641'!$N$6:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.013321130770795</c:v>
+                  <c:v>0.672134508919418</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.681088100608297</c:v>
+                  <c:v>0.569690649982621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.577279573629939</c:v>
+                  <c:v>0.497043214556482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.503664392216326</c:v>
+                  <c:v>0.376810483561959</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.381830025289294</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.31888</c:v>
+                  <c:v>0.314688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2072,29 +2036,26 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2134,11 +2095,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2062569048"/>
-        <c:axId val="2062575032"/>
+        <c:axId val="2093456024"/>
+        <c:axId val="2093462376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2062569048"/>
+        <c:axId val="2093456024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2165,11 +2126,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>N</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>úmero de processos</a:t>
+                  <a:t>Número de processos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2228,7 +2185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2062575032"/>
+        <c:crossAx val="2093462376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2236,7 +2193,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2062575032"/>
+        <c:axId val="2093462376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2330,7 +2287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2062569048"/>
+        <c:crossAx val="2093456024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2682,11 +2639,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2138654168"/>
-        <c:axId val="2108961480"/>
+        <c:axId val="2093521128"/>
+        <c:axId val="2093527560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2138654168"/>
+        <c:axId val="2093521128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2772,7 +2729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108961480"/>
+        <c:crossAx val="2093527560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2780,7 +2737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108961480"/>
+        <c:axId val="2093527560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2874,7 +2831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138654168"/>
+        <c:crossAx val="2093521128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3140,11 +3097,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109301080"/>
-        <c:axId val="2118944168"/>
+        <c:axId val="2093566808"/>
+        <c:axId val="2093573224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109301080"/>
+        <c:axId val="2093566808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3171,13 +3128,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>N</a:t>
+                  <a:t>Número de processos</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>úmero de processos</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3235,7 +3187,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118944168"/>
+        <c:crossAx val="2093573224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3243,7 +3195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118944168"/>
+        <c:axId val="2093573224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3337,7 +3289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109301080"/>
+        <c:crossAx val="2093566808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3614,11 +3566,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133372056"/>
-        <c:axId val="-2133368920"/>
+        <c:axId val="2093620872"/>
+        <c:axId val="2093627144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133372056"/>
+        <c:axId val="2093620872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3704,7 +3656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133368920"/>
+        <c:crossAx val="2093627144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3712,7 +3664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133368920"/>
+        <c:axId val="2093627144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3806,7 +3758,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133372056"/>
+        <c:crossAx val="2093620872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4072,11 +4024,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2122982280"/>
-        <c:axId val="2128649784"/>
+        <c:axId val="2093667848"/>
+        <c:axId val="2093674264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2122982280"/>
+        <c:axId val="2093667848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4103,13 +4055,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>N</a:t>
+                  <a:t>Número de processos</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>úmero de processos</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4167,7 +4114,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128649784"/>
+        <c:crossAx val="2093674264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4175,7 +4122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128649784"/>
+        <c:axId val="2093674264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4269,7 +4216,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122982280"/>
+        <c:crossAx val="2093667848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6501,13 +6448,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>68261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6566,13 +6513,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>68261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7050,10 +6997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R12"/>
+  <dimension ref="B1:R11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7134,39 +7081,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="5.25" customHeight="1" thickBot="1"/>
+    <row r="5" spans="2:18" ht="5.25" customHeight="1"/>
     <row r="6" spans="2:18">
-      <c r="B6" s="8">
-        <v>1</v>
+      <c r="B6" s="9">
+        <v>2</v>
       </c>
       <c r="D6" s="2">
-        <v>2.6457999999999999E-2</v>
+        <v>1.0070000000000001E-2</v>
       </c>
       <c r="E6" s="2">
-        <v>2.2207000000000001E-2</v>
+        <v>9.8340000000000007E-3</v>
       </c>
       <c r="F6" s="2">
         <v>9.9649999999999999E-3</v>
       </c>
       <c r="G6" s="2">
-        <v>2.1801999999999998E-2</v>
+        <v>9.9550000000000003E-3</v>
       </c>
       <c r="H6" s="2">
-        <v>2.2218999999999999E-2</v>
+        <v>1.0177E-2</v>
       </c>
       <c r="J6" s="2">
-        <f>AVERAGE(D6:H6)</f>
-        <v>2.0530200000000002E-2</v>
+        <f t="shared" ref="J6:J11" si="0">AVERAGE(D6:H6)</f>
+        <v>1.0000199999999999E-2</v>
       </c>
       <c r="K6" s="2">
-        <f>MIN(D6:H6)</f>
-        <v>9.9649999999999999E-3</v>
+        <f t="shared" ref="K6:K11" si="1">MIN(D6:H6)</f>
+        <v>9.8340000000000007E-3</v>
       </c>
       <c r="M6" s="2">
         <f>K6</f>
-        <v>9.9649999999999999E-3</v>
+        <v>9.8340000000000007E-3</v>
       </c>
       <c r="N6" s="3">
+        <f>1</f>
         <v>1</v>
       </c>
       <c r="O6" s="1">
@@ -7184,38 +7132,38 @@
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2">
-        <v>1.0070000000000001E-2</v>
+        <v>1.5094E-2</v>
       </c>
       <c r="E7" s="2">
-        <v>9.8340000000000007E-3</v>
+        <v>1.4631E-2</v>
       </c>
       <c r="F7" s="2">
-        <v>9.9649999999999999E-3</v>
+        <v>1.5200999999999999E-2</v>
       </c>
       <c r="G7" s="2">
-        <v>9.9550000000000003E-3</v>
+        <v>1.4888E-2</v>
       </c>
       <c r="H7" s="2">
-        <v>1.0177E-2</v>
+        <v>1.5075E-2</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" ref="J7:J12" si="0">AVERAGE(D7:H7)</f>
-        <v>1.0000199999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.4977799999999999E-2</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" ref="K7:K12" si="1">MIN(D7:H7)</f>
-        <v>9.8340000000000007E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.4631E-2</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" ref="M7:M12" si="2">$M$6/B7</f>
-        <v>4.9824999999999999E-3</v>
+        <f>$M$6/2</f>
+        <v>4.9170000000000004E-3</v>
       </c>
       <c r="N7" s="3">
         <f>$K$6/K7</f>
-        <v>1.0133211307707952</v>
+        <v>0.67213450891941773</v>
       </c>
       <c r="O7" s="1">
         <v>2</v>
@@ -7223,38 +7171,38 @@
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
-        <v>1.5094E-2</v>
+        <v>1.7262E-2</v>
       </c>
       <c r="E8" s="2">
-        <v>1.4631E-2</v>
+        <v>1.7357999999999998E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>1.5200999999999999E-2</v>
+        <v>1.7760999999999999E-2</v>
       </c>
       <c r="G8" s="2">
-        <v>1.4888E-2</v>
+        <v>1.7416999999999998E-2</v>
       </c>
       <c r="H8" s="2">
-        <v>1.5075E-2</v>
+        <v>1.7309000000000001E-2</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4977799999999999E-2</v>
+        <v>1.74214E-2</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>1.4631E-2</v>
+        <v>1.7262E-2</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="2"/>
-        <v>2.49125E-3</v>
+        <f>$M$6/4</f>
+        <v>2.4585000000000002E-3</v>
       </c>
       <c r="N8" s="3">
         <f>$K$6/K8</f>
-        <v>0.6810881006082975</v>
+        <v>0.56969064998262087</v>
       </c>
       <c r="O8" s="1">
         <v>4</v>
@@ -7262,38 +7210,38 @@
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="9">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2">
-        <v>1.7262E-2</v>
+        <v>2.0660999999999999E-2</v>
       </c>
       <c r="E9" s="2">
-        <v>1.7357999999999998E-2</v>
+        <v>2.0701000000000001E-2</v>
       </c>
       <c r="F9" s="2">
-        <v>1.7760999999999999E-2</v>
+        <v>2.0586E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>1.7416999999999998E-2</v>
+        <v>1.9785000000000001E-2</v>
       </c>
       <c r="H9" s="2">
-        <v>1.7309000000000001E-2</v>
+        <v>2.0704E-2</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>1.74214E-2</v>
+        <v>2.0487399999999999E-2</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>1.7262E-2</v>
+        <v>1.9785000000000001E-2</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="2"/>
-        <v>1.245625E-3</v>
+        <f>$M$6/8</f>
+        <v>1.2292500000000001E-3</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" ref="N9:N12" si="3">$K$6/K9</f>
-        <v>0.57727957362993865</v>
+        <f>$K$6/K9</f>
+        <v>0.4970432145564822</v>
       </c>
       <c r="O9" s="1">
         <v>8</v>
@@ -7301,110 +7249,74 @@
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="9">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2">
-        <v>2.0660999999999999E-2</v>
+        <v>2.8215E-2</v>
       </c>
       <c r="E10" s="2">
-        <v>2.0701000000000001E-2</v>
+        <v>0.75236599999999998</v>
       </c>
       <c r="F10" s="2">
-        <v>2.0586E-2</v>
+        <v>2.6098E-2</v>
       </c>
       <c r="G10" s="2">
-        <v>1.9785000000000001E-2</v>
+        <v>0.77610699999999999</v>
       </c>
       <c r="H10" s="2">
-        <v>2.0704E-2</v>
+        <v>2.7480000000000001E-2</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>2.0487399999999999E-2</v>
+        <v>0.32205319999999998</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="1"/>
-        <v>1.9785000000000001E-2</v>
+        <v>2.6098E-2</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="2"/>
-        <v>6.2281249999999999E-4</v>
+        <f>$M$6/12</f>
+        <v>8.1950000000000002E-4</v>
       </c>
       <c r="N10" s="3">
-        <f t="shared" si="3"/>
-        <v>0.50366439221632553</v>
+        <f>$K$6/K10</f>
+        <v>0.37681048356195879</v>
       </c>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="9">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2">
-        <v>2.8215E-2</v>
+        <v>29.229883999999998</v>
       </c>
       <c r="E11" s="2">
-        <v>0.75236599999999998</v>
+        <v>19.990462999999998</v>
       </c>
       <c r="F11" s="2">
-        <v>2.6098E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>0.77610699999999999</v>
+        <v>30.259924999999999</v>
       </c>
       <c r="H11" s="2">
-        <v>2.7480000000000001E-2</v>
+        <v>28.109921</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>0.32205319999999998</v>
+        <v>21.524288599999998</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>2.6098E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="2"/>
-        <v>4.1520833333333335E-4</v>
+        <f>$M$6/16</f>
+        <v>6.1462500000000005E-4</v>
       </c>
       <c r="N11" s="3">
-        <f t="shared" si="3"/>
-        <v>0.38183002528929422</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18">
-      <c r="B12" s="9">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2">
-        <v>29.229883999999998</v>
-      </c>
-      <c r="E12" s="2">
-        <v>19.990462999999998</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <v>30.259924999999999</v>
-      </c>
-      <c r="H12" s="2">
-        <v>28.109921</v>
-      </c>
-      <c r="J12" s="2">
-        <f t="shared" si="0"/>
-        <v>21.524288599999998</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" si="1"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="M12" s="2">
-        <f t="shared" si="2"/>
-        <v>3.1140625E-4</v>
-      </c>
-      <c r="N12" s="3">
-        <f t="shared" si="3"/>
-        <v>0.31888</v>
+        <f>$K$6/K11</f>
+        <v>0.31468800000000002</v>
       </c>
     </row>
   </sheetData>
@@ -7427,7 +7339,7 @@
   <dimension ref="A2:W39"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7516,7 +7428,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:23" ht="16" thickBot="1">
+    <row r="5" spans="1:23">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -7543,40 +7455,41 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="1"/>
-      <c r="B6" s="8">
-        <v>1</v>
+      <c r="B6" s="9">
+        <v>2</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2">
-        <v>2.6457999999999999E-2</v>
+        <v>1.1254E-2</v>
       </c>
       <c r="E6" s="2">
-        <v>2.2207000000000001E-2</v>
+        <v>1.1173000000000001E-2</v>
       </c>
       <c r="F6" s="2">
-        <v>9.9649999999999999E-3</v>
+        <v>1.1055000000000001E-2</v>
       </c>
       <c r="G6" s="2">
-        <v>2.1801999999999998E-2</v>
+        <v>1.1138E-2</v>
       </c>
       <c r="H6" s="2">
-        <v>2.2218999999999999E-2</v>
+        <v>1.1514E-2</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2">
-        <f>AVERAGE(D6:H6)</f>
-        <v>2.0530200000000002E-2</v>
+        <f t="shared" ref="J6:J11" si="0">AVERAGE(D6:H6)</f>
+        <v>1.12268E-2</v>
       </c>
       <c r="K6" s="2">
-        <f>MIN(D6:H6)</f>
-        <v>9.9649999999999999E-3</v>
+        <f t="shared" ref="K6:K11" si="1">MIN(D6:H6)</f>
+        <v>1.1055000000000001E-2</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="2">
         <f>K6</f>
-        <v>9.9649999999999999E-3</v>
+        <v>1.1055000000000001E-2</v>
       </c>
       <c r="N6" s="3">
+        <f>1</f>
         <v>1</v>
       </c>
       <c r="O6" s="1">
@@ -7600,41 +7513,41 @@
     <row r="7" spans="1:23">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="2">
-        <v>1.1254E-2</v>
+        <v>1.7632999999999999E-2</v>
       </c>
       <c r="E7" s="2">
-        <v>1.1173000000000001E-2</v>
+        <v>1.7093000000000001E-2</v>
       </c>
       <c r="F7" s="2">
-        <v>1.1055000000000001E-2</v>
+        <v>1.6853E-2</v>
       </c>
       <c r="G7" s="2">
-        <v>1.1138E-2</v>
+        <v>1.6815E-2</v>
       </c>
       <c r="H7" s="2">
-        <v>1.1514E-2</v>
+        <v>1.6709999999999999E-2</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2">
-        <f t="shared" ref="J7:J12" si="0">AVERAGE(D7:H7)</f>
-        <v>1.12268E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.7020799999999999E-2</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" ref="K7:K12" si="1">MIN(D7:H7)</f>
-        <v>1.1055000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.6709999999999999E-2</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="2">
-        <f t="shared" ref="M7:M12" si="2">$M$6/B7</f>
-        <v>4.9824999999999999E-3</v>
+        <f>$M$6/2</f>
+        <v>5.5275000000000003E-3</v>
       </c>
       <c r="N7" s="3">
         <f>$K$6/K7</f>
-        <v>0.90140208050655801</v>
+        <v>0.66157989228007186</v>
       </c>
       <c r="O7" s="1">
         <v>2</v>
@@ -7651,41 +7564,41 @@
     <row r="8" spans="1:23">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2">
-        <v>1.7632999999999999E-2</v>
+        <v>2.0275999999999999E-2</v>
       </c>
       <c r="E8" s="2">
-        <v>1.7093000000000001E-2</v>
+        <v>1.9903000000000001E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>1.6853E-2</v>
+        <v>2.2898999999999999E-2</v>
       </c>
       <c r="G8" s="2">
-        <v>1.6815E-2</v>
+        <v>1.9255000000000001E-2</v>
       </c>
       <c r="H8" s="2">
-        <v>1.6709999999999999E-2</v>
+        <v>1.9460000000000002E-2</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>1.7020799999999999E-2</v>
+        <v>2.0358599999999998E-2</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>1.6709999999999999E-2</v>
+        <v>1.9255000000000001E-2</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="2">
-        <f t="shared" si="2"/>
-        <v>2.49125E-3</v>
+        <f>$M$6/4</f>
+        <v>2.7637500000000001E-3</v>
       </c>
       <c r="N8" s="3">
         <f>$K$6/K8</f>
-        <v>0.59634949132256132</v>
+        <v>0.57413658789924693</v>
       </c>
       <c r="O8" s="1">
         <v>4</v>
@@ -7702,45 +7615,43 @@
     <row r="9" spans="1:23">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2">
-        <v>2.0275999999999999E-2</v>
+        <v>2.3469E-2</v>
       </c>
       <c r="E9" s="2">
-        <v>1.9903000000000001E-2</v>
+        <v>2.3827000000000001E-2</v>
       </c>
       <c r="F9" s="2">
-        <v>2.2898999999999999E-2</v>
+        <v>2.4065E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>1.9255000000000001E-2</v>
+        <v>2.4671999999999999E-2</v>
       </c>
       <c r="H9" s="2">
-        <v>1.9460000000000002E-2</v>
+        <v>2.4181000000000001E-2</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>2.0358599999999998E-2</v>
+        <v>2.4042800000000003E-2</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>1.9255000000000001E-2</v>
+        <v>2.3469E-2</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="2">
-        <f t="shared" si="2"/>
-        <v>1.245625E-3</v>
+        <f>$M$6/8</f>
+        <v>1.3818750000000001E-3</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" ref="N9:N12" si="3">$K$6/K9</f>
-        <v>0.51752791482731753</v>
-      </c>
-      <c r="O9" s="1">
-        <v>8</v>
-      </c>
+        <f>$K$6/K9</f>
+        <v>0.47104691294899659</v>
+      </c>
+      <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -7753,41 +7664,41 @@
     <row r="10" spans="1:23">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2">
-        <v>2.3469E-2</v>
+        <v>2.7639E-2</v>
       </c>
       <c r="E10" s="2">
-        <v>2.3827000000000001E-2</v>
+        <v>2.6969E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>2.4065E-2</v>
+        <v>2.8320000000000001E-2</v>
       </c>
       <c r="G10" s="2">
-        <v>2.4671999999999999E-2</v>
+        <v>2.6971999999999999E-2</v>
       </c>
       <c r="H10" s="2">
-        <v>2.4181000000000001E-2</v>
+        <v>2.7817000000000001E-2</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>2.4042800000000003E-2</v>
+        <v>2.7543400000000003E-2</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="1"/>
-        <v>2.3469E-2</v>
+        <v>2.6969E-2</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="2">
-        <f t="shared" si="2"/>
-        <v>6.2281249999999999E-4</v>
+        <f>$M$6/12</f>
+        <v>9.2125000000000009E-4</v>
       </c>
       <c r="N10" s="3">
-        <f t="shared" si="3"/>
-        <v>0.42460266734841706</v>
+        <f>$K$6/K10</f>
+        <v>0.4099150876932775</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -7802,41 +7713,41 @@
     <row r="11" spans="1:23">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2">
-        <v>2.7639E-2</v>
+        <v>7.4031E-2</v>
       </c>
       <c r="E11" s="2">
-        <v>2.6969E-2</v>
+        <v>3.3123E-2</v>
       </c>
       <c r="F11" s="2">
-        <v>2.8320000000000001E-2</v>
+        <v>3.3031999999999999E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>2.6971999999999999E-2</v>
+        <v>3.4818000000000002E-2</v>
       </c>
       <c r="H11" s="2">
-        <v>2.7817000000000001E-2</v>
+        <v>4.4824000000000003E-2</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>2.7543400000000003E-2</v>
+        <v>4.3965600000000001E-2</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>2.6969E-2</v>
+        <v>3.3031999999999999E-2</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="2">
-        <f t="shared" si="2"/>
-        <v>4.1520833333333335E-4</v>
+        <f>$M$6/16</f>
+        <v>6.9093750000000004E-4</v>
       </c>
       <c r="N11" s="3">
-        <f t="shared" si="3"/>
-        <v>0.36949831287774854</v>
+        <f>$K$6/K11</f>
+        <v>0.33467546621457983</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -7850,43 +7761,19 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="1"/>
-      <c r="B12" s="9">
-        <v>32</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="2">
-        <v>7.4031E-2</v>
-      </c>
-      <c r="E12" s="2">
-        <v>3.3123E-2</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3.3031999999999999E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <v>3.4818000000000002E-2</v>
-      </c>
-      <c r="H12" s="2">
-        <v>4.4824000000000003E-2</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="2">
-        <f t="shared" si="0"/>
-        <v>4.3965600000000001E-2</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" si="1"/>
-        <v>3.3031999999999999E-2</v>
-      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="2">
-        <f t="shared" si="2"/>
-        <v>3.1140625E-4</v>
-      </c>
-      <c r="N12" s="3">
-        <f t="shared" si="3"/>
-        <v>0.30167716154032453</v>
-      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -8549,20 +8436,6 @@
     </row>
     <row r="39" spans="1:23">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -8963,7 +8836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Graficos lvl1 e ram
</commit_message>
<xml_diff>
--- a/gráficos.xlsx
+++ b/gráficos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="714" activeTab="2"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="25260" windowHeight="14800" tabRatio="714"/>
   </bookViews>
   <sheets>
     <sheet name="19KBytes-641" sheetId="6" r:id="rId1"/>
@@ -245,7 +245,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="100">
+  <cellStyleXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -346,6 +346,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -411,7 +469,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="100">
+  <cellStyles count="158">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -461,6 +519,35 @@
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -510,6 +597,35 @@
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="79"/>
   </cellStyles>
@@ -583,17 +699,11 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:tx>
+            <c:v>Tempo de execução</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -602,26 +712,29 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -629,26 +742,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$K$6:$K$11</c:f>
+              <c:f>'19KBytes-641'!$K$6:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>0.020305</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.009834</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.014631</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.017262</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.019785</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.026098</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.03125</c:v>
                 </c:pt>
               </c:numCache>
@@ -657,10 +773,16 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo ideal</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
               <a:prstDash val="sysDot"/>
             </a:ln>
           </c:spPr>
@@ -672,26 +794,29 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -699,27 +824,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$M$6:$M$11</c:f>
+              <c:f>'19KBytes-641'!$M$6:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.009834</c:v>
+                  <c:v>0.020305</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.004917</c:v>
+                  <c:v>0.0101525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0024585</c:v>
+                  <c:v>0.00507625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00122925</c:v>
+                  <c:v>0.002538125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0008195</c:v>
+                  <c:v>0.0012690625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.000614625</c:v>
+                  <c:v>0.000846041666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00063453125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,19 +857,19 @@
         <c:dLbls>
           <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
+          <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2101860168"/>
-        <c:axId val="2101875608"/>
+        <c:axId val="2085949928"/>
+        <c:axId val="2085957192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2101860168"/>
+        <c:axId val="2085949928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,8 +905,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.502586106799167"/>
-              <c:y val="0.921363306687398"/>
+              <c:x val="0.404969835637742"/>
+              <c:y val="0.824458908040861"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -827,7 +955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101875608"/>
+        <c:crossAx val="2085957192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -835,7 +963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101875608"/>
+        <c:axId val="2085957192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +1057,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101860168"/>
+        <c:crossAx val="2085949928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -941,6 +1069,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1035,82 +1168,11 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'19KBytes-641'!$N$6:$N$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.672134508919418</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.569690649982621</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.497043214556482</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.376810483561959</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.314688</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo ideal</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="38100" cmpd="sng">
               <a:prstDash val="sysDot"/>
@@ -1128,26 +1190,29 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
+              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1170,6 +1235,80 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo de execução</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'19KBytes-641'!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'19KBytes-641'!$N$6:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.064775269473256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.387806711776365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.17628316533426</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.026282537275714</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.778028967736991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1187,11 +1326,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2101952408"/>
-        <c:axId val="2101958776"/>
+        <c:axId val="2086031784"/>
+        <c:axId val="2086038168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2101952408"/>
+        <c:axId val="2086031784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,8 +1366,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.502893519168512"/>
-              <c:y val="0.90805335017283"/>
+              <c:x val="0.421789079643733"/>
+              <c:y val="0.776905977855157"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1277,7 +1416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101958776"/>
+        <c:crossAx val="2086038168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1285,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101958776"/>
+        <c:axId val="2086038168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,7 +1487,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1379,7 +1518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101952408"/>
+        <c:crossAx val="2086031784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1391,6 +1530,20 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.37408463717704"/>
+          <c:y val="0.881193405781484"/>
+          <c:w val="0.402566562268586"/>
+          <c:h val="0.0849620731501354"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1485,10 +1638,90 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Tempo de execução</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'19KBytes-662'!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'19KBytes-662'!$K$6:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.025379</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.011055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.019255</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.023469</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.026969</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.033032</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo ideal</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="38100" cmpd="sng">
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
               <a:prstDash val="sysDot"/>
             </a:ln>
           </c:spPr>
@@ -1500,26 +1733,29 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'19KBytes-662'!$B$6:$B$11</c:f>
+              <c:f>'19KBytes-662'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1527,101 +1763,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-662'!$M$6:$M$11</c:f>
+              <c:f>'19KBytes-662'!$M$6:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.011055</c:v>
+                  <c:v>0.025379</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0055275</c:v>
+                  <c:v>0.0126895</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00276375</c:v>
+                  <c:v>0.00634475</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.001381875</c:v>
+                  <c:v>0.003172375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00092125</c:v>
+                  <c:v>0.0015861875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0006909375</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>'19KBytes-662'!$B$6:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'19KBytes-662'!$K$6:$K$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.011055</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.01671</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.019255</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.023469</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.026969</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.033032</c:v>
+                  <c:v>0.00105745833333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00079309375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1639,11 +1804,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102008328"/>
-        <c:axId val="2102014520"/>
+        <c:axId val="2086087048"/>
+        <c:axId val="2085127304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102008328"/>
+        <c:axId val="2086087048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1679,8 +1844,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.502586106799167"/>
-              <c:y val="0.921363306687398"/>
+              <c:x val="0.425404930507848"/>
+              <c:y val="0.826083126809773"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1729,7 +1894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102014520"/>
+        <c:crossAx val="2085127304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1737,7 +1902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102014520"/>
+        <c:axId val="2085127304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,7 +1996,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102008328"/>
+        <c:crossAx val="2086087048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1843,6 +2008,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1939,14 +2109,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Tempo de execução</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1954,56 +2127,32 @@
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$N$6:$N$11</c:f>
+              <c:f>'19KBytes-662'!$N$6:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.672134508919418</c:v>
+                  <c:v>2.295703301673451</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.569690649982621</c:v>
+                  <c:v>1.518791143028127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.497043214556482</c:v>
+                  <c:v>1.31804726045183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.376810483561959</c:v>
+                  <c:v>1.081383953300098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.314688</c:v>
+                  <c:v>0.941043420223219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.768315572777912</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2013,54 +2162,29 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo ideal</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="38100" cmpd="sng">
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
               <a:prstDash val="sysDot"/>
             </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-          </c:dPt>
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'19KBytes-641'!$B$6:$B$11</c:f>
+              <c:f>'19KBytes-662'!$O$6:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'19KBytes-641'!$O$6:$O$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2089,11 +2213,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102055464"/>
-        <c:axId val="2102061800"/>
+        <c:axId val="2085194392"/>
+        <c:axId val="2085200776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102055464"/>
+        <c:axId val="2085194392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2129,8 +2253,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.502893519168512"/>
-              <c:y val="0.90805335017283"/>
+              <c:x val="0.418033394331012"/>
+              <c:y val="0.797107354602558"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2179,7 +2303,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102061800"/>
+        <c:crossAx val="2085200776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2187,7 +2311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102061800"/>
+        <c:axId val="2085200776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2250,7 +2374,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2281,7 +2405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102055464"/>
+        <c:crossAx val="2085194392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2293,6 +2417,20 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.388200669708957"/>
+          <c:y val="0.888725471996276"/>
+          <c:w val="0.449927334300184"/>
+          <c:h val="0.0795756721265034"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2394,46 +2532,39 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="0"/>
           <c:tx>
-            <c:v>Series 2</c:v>
+            <c:v>Tempo de execução</c:v>
           </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'RAM-641'!$B$6:$B$11</c:f>
+              <c:f>'RAM-641'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2441,102 +2572,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RAM-641'!$R$6:$R$11</c:f>
+              <c:f>'RAM-641'!$P$6:$P$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>480.461862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>184.807517</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>92.4037585</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>46.20187925</c:v>
+                  <c:v>102.575956</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.100939625</c:v>
+                  <c:v>79.235024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.40062641666667</c:v>
+                  <c:v>75.93078800000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.5504698125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Tempo ideal</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'RAM-641'!$B$6:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RAM-641'!$R$6:$R$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>184.807517</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>92.4037585</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>46.20187925</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23.100939625</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.40062641666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.5504698125</c:v>
+                  <c:v>88.001002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>189.693415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2545,32 +2604,46 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'RAM-641'!$B$6:$B$11</c:f>
+              <c:f>'RAM-641'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2578,27 +2651,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RAM-641'!$P$6:$P$11</c:f>
+              <c:f>'RAM-641'!$R$6:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>184.807517</c:v>
+                  <c:v>480.461862</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102.575956</c:v>
+                  <c:v>240.230931</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.235024</c:v>
+                  <c:v>120.1154655</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.93078800000001</c:v>
+                  <c:v>60.05773275</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.001002</c:v>
+                  <c:v>30.028866375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>189.693415</c:v>
+                  <c:v>20.01924425</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.0144331875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2615,11 +2691,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102120824"/>
-        <c:axId val="2102127256"/>
+        <c:axId val="2086133944"/>
+        <c:axId val="2086140376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102120824"/>
+        <c:axId val="2086133944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2655,8 +2731,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.498180789018831"/>
-              <c:y val="0.925694134228118"/>
+              <c:x val="0.44398436458145"/>
+              <c:y val="0.805562756672184"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2705,7 +2781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102127256"/>
+        <c:crossAx val="2086140376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2713,7 +2789,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102127256"/>
+        <c:axId val="2086140376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2807,7 +2883,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102120824"/>
+        <c:crossAx val="2086133944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2819,6 +2895,20 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.408215410785357"/>
+          <c:y val="0.909590202434966"/>
+          <c:w val="0.351204099111247"/>
+          <c:h val="0.0753933755704688"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2917,82 +3007,11 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Sem flags</c:v>
+            <c:v>Tempo ideal</c:v>
           </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'RAM-641'!$B$6:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RAM-641'!$S$6:$S$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.801665070516135</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.332396807250288</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.433894364430934</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.100061508390552</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.97424318603785</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:spPr>
             <a:ln w="38100" cmpd="sng">
               <a:prstDash val="sysDot"/>
@@ -3003,26 +3022,29 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'RAM-641'!$B$6:$B$11</c:f>
+              <c:f>'RAM-641'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3045,6 +3067,77 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo de execução</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'RAM-641'!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RAM-641'!$S$6:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.59979610028525</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.683961824347998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.063756123807068</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.327629077153788</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.459731719872916</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.532833635790678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3061,11 +3154,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102166120"/>
-        <c:axId val="2102172520"/>
+        <c:axId val="2086179192"/>
+        <c:axId val="2086185576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102166120"/>
+        <c:axId val="2086179192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3101,8 +3194,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.485596046556236"/>
-              <c:y val="0.929752234843918"/>
+              <c:x val="0.443267971010704"/>
+              <c:y val="0.845013367796877"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3151,7 +3244,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102172520"/>
+        <c:crossAx val="2086185576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3159,7 +3252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102172520"/>
+        <c:axId val="2086185576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3222,7 +3315,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3253,7 +3346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102166120"/>
+        <c:crossAx val="2086179192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3265,6 +3358,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3366,8 +3464,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0757685055837173"/>
-          <c:y val="0.139465320259595"/>
+          <c:x val="0.0757684996004755"/>
+          <c:y val="0.0803592620964852"/>
           <c:w val="0.908895140285924"/>
           <c:h val="0.694052280422254"/>
         </c:manualLayout>
@@ -3376,33 +3474,39 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Tempo de execução</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'RAM-662'!$B$6:$B$11</c:f>
+              <c:f>'RAM-662'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3410,26 +3514,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RAM-662'!$P$6:$P$11</c:f>
+              <c:f>'RAM-662'!$P$6:$P$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>649.431485</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>197.507382</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>93.552012</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>62.926752</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>48.366109</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45.371532</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>62.674204</c:v>
                 </c:pt>
               </c:numCache>
@@ -3438,15 +3545,17 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo ideal</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd" cmpd="sng">
+            <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:prstDash val="sysDot"/>
-              <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -3454,26 +3563,29 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'RAM-662'!$B$6:$B$11</c:f>
+              <c:f>'RAM-662'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3481,27 +3593,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RAM-662'!$R$6:$R$11</c:f>
+              <c:f>'RAM-662'!$R$6:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>197.507382</c:v>
+                  <c:v>649.431485</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.753691</c:v>
+                  <c:v>324.7157425</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.3768455</c:v>
+                  <c:v>162.35787125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.68842275</c:v>
+                  <c:v>81.17893562499999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.4589485</c:v>
+                  <c:v>40.5894678125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.344211375</c:v>
+                  <c:v>27.05964520833333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.29473390625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3518,11 +3633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102220712"/>
-        <c:axId val="2102226984"/>
+        <c:axId val="2086233768"/>
+        <c:axId val="2086240040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102220712"/>
+        <c:axId val="2086233768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3558,8 +3673,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.498180789018831"/>
-              <c:y val="0.925694134228118"/>
+              <c:x val="0.426583333829725"/>
+              <c:y val="0.842930456903348"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3608,7 +3723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102226984"/>
+        <c:crossAx val="2086240040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3616,7 +3731,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102226984"/>
+        <c:axId val="2086240040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3710,7 +3825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102220712"/>
+        <c:crossAx val="2086233768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3722,6 +3837,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3815,7 +3935,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0698058209594512"/>
+          <c:y val="0.0817506841800096"/>
+          <c:w val="0.911076529768009"/>
+          <c:h val="0.733669390576594"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -3823,42 +3953,45 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Sem flags</c:v>
+            <c:v>Tempo de execução</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'RAM-641'!$B$6:$B$11</c:f>
+              <c:f>'RAM-641'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3866,27 +3999,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RAM-641'!$S$6:$S$11</c:f>
+              <c:f>'RAM-662'!$S$6:$S$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.801665070516135</c:v>
+                  <c:v>3.288137782110847</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.332396807250288</c:v>
+                  <c:v>6.94192964016637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.433894364430934</c:v>
+                  <c:v>10.32043549617816</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.100061508390552</c:v>
+                  <c:v>13.42740812580148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.97424318603785</c:v>
+                  <c:v>14.31363360179242</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.3620220689201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3896,8 +4032,11 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Tempo ideal</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="38100" cmpd="sng">
+            <a:ln>
               <a:prstDash val="sysDot"/>
             </a:ln>
           </c:spPr>
@@ -3906,26 +4045,29 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'RAM-641'!$B$6:$B$11</c:f>
+              <c:f>'RAM-641'!$B$6:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3933,10 +4075,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RAM-641'!$T$6:$T$9</c:f>
+              <c:f>'RAM-662'!$T$6:$T$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -3948,6 +4090,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3964,11 +4109,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102267368"/>
-        <c:axId val="2102273768"/>
+        <c:axId val="2086280808"/>
+        <c:axId val="2086287208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102267368"/>
+        <c:axId val="2086280808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4004,8 +4149,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.485596046556236"/>
-              <c:y val="0.929752234843918"/>
+              <c:x val="0.444419574388557"/>
+              <c:y val="0.887046528083686"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4054,7 +4199,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102273768"/>
+        <c:crossAx val="2086287208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4062,7 +4207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102273768"/>
+        <c:axId val="2086287208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4125,7 +4270,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4156,7 +4301,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102267368"/>
+        <c:crossAx val="2086280808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4168,6 +4313,20 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.394164821001021"/>
+          <c:y val="0.938738927860982"/>
+          <c:w val="0.343069632129415"/>
+          <c:h val="0.0612610721390179"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -6387,15 +6546,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>68261</xdr:rowOff>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>93661</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6416,16 +6575,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>568325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>150811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>130174</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6451,16 +6610,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>68261</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>169861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>149224</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6483,16 +6642,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>758825</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>112711</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>739775</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6591,10 +6750,10 @@
       <xdr:rowOff>96836</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>685799</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6937,10 +7096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R11"/>
+  <dimension ref="B1:R12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7023,38 +7182,37 @@
     </row>
     <row r="5" spans="2:18" ht="5.25" customHeight="1"/>
     <row r="6" spans="2:18">
-      <c r="B6" s="9">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.0070000000000001E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>9.8340000000000007E-3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>9.9649999999999999E-3</v>
-      </c>
-      <c r="G6" s="2">
-        <v>9.9550000000000003E-3</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1.0177E-2</v>
-      </c>
-      <c r="J6" s="2">
-        <f t="shared" ref="J6:J11" si="0">AVERAGE(D6:H6)</f>
-        <v>1.0000199999999999E-2</v>
-      </c>
-      <c r="K6" s="2">
-        <f t="shared" ref="K6:K11" si="1">MIN(D6:H6)</f>
-        <v>9.8340000000000007E-3</v>
-      </c>
-      <c r="M6" s="2">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.2495000000000001E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.2637000000000001E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.3025E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.0305E-2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.3372E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <f>AVERAGE(D6:H6)</f>
+        <v>2.2366800000000003E-2</v>
+      </c>
+      <c r="K6" s="1">
+        <f>MIN(D6:H6)</f>
+        <v>2.0305E-2</v>
+      </c>
+      <c r="M6" s="1">
         <f>K6</f>
-        <v>9.8340000000000007E-3</v>
-      </c>
-      <c r="N6" s="3">
-        <f>1</f>
+        <v>2.0305E-2</v>
+      </c>
+      <c r="N6" s="1">
         <v>1</v>
       </c>
       <c r="O6" s="1">
@@ -7072,38 +7230,38 @@
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
-        <v>1.5094E-2</v>
+        <v>1.0070000000000001E-2</v>
       </c>
       <c r="E7" s="2">
-        <v>1.4631E-2</v>
+        <v>9.8340000000000007E-3</v>
       </c>
       <c r="F7" s="2">
-        <v>1.5200999999999999E-2</v>
+        <v>9.9649999999999999E-3</v>
       </c>
       <c r="G7" s="2">
-        <v>1.4888E-2</v>
+        <v>9.9550000000000003E-3</v>
       </c>
       <c r="H7" s="2">
-        <v>1.5075E-2</v>
+        <v>1.0177E-2</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="0"/>
-        <v>1.4977799999999999E-2</v>
+        <f t="shared" ref="J7:J12" si="0">AVERAGE(D7:H7)</f>
+        <v>1.0000199999999999E-2</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4631E-2</v>
+        <f t="shared" ref="K7:K12" si="1">MIN(D7:H7)</f>
+        <v>9.8340000000000007E-3</v>
       </c>
       <c r="M7" s="2">
-        <f>$M$6/2</f>
-        <v>4.9170000000000004E-3</v>
+        <f>$M$6/B7</f>
+        <v>1.01525E-2</v>
       </c>
       <c r="N7" s="3">
         <f>$K$6/K7</f>
-        <v>0.67213450891941773</v>
+        <v>2.0647752694732557</v>
       </c>
       <c r="O7" s="1">
         <v>2</v>
@@ -7111,38 +7269,38 @@
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>1.7262E-2</v>
+        <v>1.5094E-2</v>
       </c>
       <c r="E8" s="2">
-        <v>1.7357999999999998E-2</v>
+        <v>1.4631E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>1.7760999999999999E-2</v>
+        <v>1.5200999999999999E-2</v>
       </c>
       <c r="G8" s="2">
-        <v>1.7416999999999998E-2</v>
+        <v>1.4888E-2</v>
       </c>
       <c r="H8" s="2">
-        <v>1.7309000000000001E-2</v>
+        <v>1.5075E-2</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>1.74214E-2</v>
+        <v>1.4977799999999999E-2</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>1.7262E-2</v>
+        <v>1.4631E-2</v>
       </c>
       <c r="M8" s="2">
-        <f>$M$6/4</f>
-        <v>2.4585000000000002E-3</v>
+        <f>$M$6/B8</f>
+        <v>5.07625E-3</v>
       </c>
       <c r="N8" s="3">
         <f>$K$6/K8</f>
-        <v>0.56969064998262087</v>
+        <v>1.3878067117763653</v>
       </c>
       <c r="O8" s="1">
         <v>4</v>
@@ -7150,38 +7308,38 @@
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="9">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
-        <v>2.0660999999999999E-2</v>
+        <v>1.7262E-2</v>
       </c>
       <c r="E9" s="2">
-        <v>2.0701000000000001E-2</v>
+        <v>1.7357999999999998E-2</v>
       </c>
       <c r="F9" s="2">
-        <v>2.0586E-2</v>
+        <v>1.7760999999999999E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>1.9785000000000001E-2</v>
+        <v>1.7416999999999998E-2</v>
       </c>
       <c r="H9" s="2">
-        <v>2.0704E-2</v>
+        <v>1.7309000000000001E-2</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>2.0487399999999999E-2</v>
+        <v>1.74214E-2</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>1.9785000000000001E-2</v>
+        <v>1.7262E-2</v>
       </c>
       <c r="M9" s="2">
-        <f>$M$6/8</f>
-        <v>1.2292500000000001E-3</v>
+        <f>$M$6/B9</f>
+        <v>2.538125E-3</v>
       </c>
       <c r="N9" s="3">
         <f>$K$6/K9</f>
-        <v>0.4970432145564822</v>
+        <v>1.1762831653342603</v>
       </c>
       <c r="O9" s="1">
         <v>8</v>
@@ -7189,74 +7347,110 @@
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="9">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2">
-        <v>2.8215E-2</v>
+        <v>2.0660999999999999E-2</v>
       </c>
       <c r="E10" s="2">
-        <v>0.75236599999999998</v>
+        <v>2.0701000000000001E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>2.6098E-2</v>
+        <v>2.0586E-2</v>
       </c>
       <c r="G10" s="2">
-        <v>0.77610699999999999</v>
+        <v>1.9785000000000001E-2</v>
       </c>
       <c r="H10" s="2">
-        <v>2.7480000000000001E-2</v>
+        <v>2.0704E-2</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>0.32205319999999998</v>
+        <v>2.0487399999999999E-2</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="1"/>
-        <v>2.6098E-2</v>
+        <v>1.9785000000000001E-2</v>
       </c>
       <c r="M10" s="2">
-        <f>$M$6/12</f>
-        <v>8.1950000000000002E-4</v>
+        <f>$M$6/B10</f>
+        <v>1.2690625E-3</v>
       </c>
       <c r="N10" s="3">
         <f>$K$6/K10</f>
-        <v>0.37681048356195879</v>
+        <v>1.0262825372757138</v>
       </c>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="9">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2">
-        <v>29.229883999999998</v>
+        <v>2.8215E-2</v>
       </c>
       <c r="E11" s="2">
-        <v>19.990462999999998</v>
+        <v>0.75236599999999998</v>
       </c>
       <c r="F11" s="2">
-        <v>3.125E-2</v>
+        <v>2.6098E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>30.259924999999999</v>
+        <v>0.77610699999999999</v>
       </c>
       <c r="H11" s="2">
-        <v>28.109921</v>
+        <v>2.7480000000000001E-2</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>21.524288599999998</v>
+        <v>0.32205319999999998</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>3.125E-2</v>
+        <v>2.6098E-2</v>
       </c>
       <c r="M11" s="2">
-        <f>$M$6/16</f>
-        <v>6.1462500000000005E-4</v>
+        <f>$M$6/B11</f>
+        <v>8.4604166666666671E-4</v>
       </c>
       <c r="N11" s="3">
         <f>$K$6/K11</f>
-        <v>0.31468800000000002</v>
+        <v>0.77802896773699137</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="9">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2">
+        <v>29.229883999999998</v>
+      </c>
+      <c r="E12" s="2">
+        <v>19.990462999999998</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>30.259924999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>28.109921</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>21.524288599999998</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="1"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M12" s="2">
+        <f>$M$6/B12</f>
+        <v>6.3453125E-4</v>
+      </c>
+      <c r="N12" s="3">
+        <f>$K$6/K12</f>
+        <v>0.64976</v>
       </c>
     </row>
   </sheetData>
@@ -7278,8 +7472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W39"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7395,41 +7589,39 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="1"/>
-      <c r="B6" s="9">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2">
-        <v>1.1254E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.1173000000000001E-2</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.1055000000000001E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1.1138E-2</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1.1514E-2</v>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2.6848E-2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>2.5378999999999999E-2</v>
+      </c>
+      <c r="F6" s="18">
+        <v>2.5458000000000001E-2</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2.5624000000000001E-2</v>
+      </c>
+      <c r="H6" s="18">
+        <v>2.5714000000000001E-2</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="2">
-        <f t="shared" ref="J6:J11" si="0">AVERAGE(D6:H6)</f>
+      <c r="J6" s="18">
+        <f>AVERAGE(D7:H7)</f>
         <v>1.12268E-2</v>
       </c>
-      <c r="K6" s="2">
-        <f t="shared" ref="K6:K11" si="1">MIN(D6:H6)</f>
-        <v>1.1055000000000001E-2</v>
+      <c r="K6" s="18">
+        <f>MIN(D6:H6)</f>
+        <v>2.5378999999999999E-2</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="2">
+      <c r="M6" s="18">
         <f>K6</f>
-        <v>1.1055000000000001E-2</v>
-      </c>
-      <c r="N6" s="3">
-        <f>1</f>
+        <v>2.5378999999999999E-2</v>
+      </c>
+      <c r="N6" s="18">
         <v>1</v>
       </c>
       <c r="O6" s="1">
@@ -7453,41 +7645,41 @@
     <row r="7" spans="1:23">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="2">
-        <v>1.7632999999999999E-2</v>
+        <v>1.1254E-2</v>
       </c>
       <c r="E7" s="2">
-        <v>1.7093000000000001E-2</v>
+        <v>1.1173000000000001E-2</v>
       </c>
       <c r="F7" s="2">
-        <v>1.6853E-2</v>
+        <v>1.1055000000000001E-2</v>
       </c>
       <c r="G7" s="2">
-        <v>1.6815E-2</v>
+        <v>1.1138E-2</v>
       </c>
       <c r="H7" s="2">
-        <v>1.6709999999999999E-2</v>
+        <v>1.1514E-2</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7020799999999999E-2</v>
+        <f>AVERAGE(D7:H7)</f>
+        <v>1.12268E-2</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6709999999999999E-2</v>
+        <f>MIN(D7:H7)</f>
+        <v>1.1055000000000001E-2</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="2">
-        <f>$M$6/2</f>
-        <v>5.5275000000000003E-3</v>
+        <f>$M$6/B7</f>
+        <v>1.2689499999999999E-2</v>
       </c>
       <c r="N7" s="3">
         <f>$K$6/K7</f>
-        <v>0.66157989228007186</v>
+        <v>2.2957033016734507</v>
       </c>
       <c r="O7" s="1">
         <v>2</v>
@@ -7504,41 +7696,41 @@
     <row r="8" spans="1:23">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2">
-        <v>2.0275999999999999E-2</v>
+        <v>1.7632999999999999E-2</v>
       </c>
       <c r="E8" s="2">
-        <v>1.9903000000000001E-2</v>
+        <v>1.7093000000000001E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>2.2898999999999999E-2</v>
+        <v>1.6853E-2</v>
       </c>
       <c r="G8" s="2">
-        <v>1.9255000000000001E-2</v>
+        <v>1.6815E-2</v>
       </c>
       <c r="H8" s="2">
-        <v>1.9460000000000002E-2</v>
+        <v>1.6709999999999999E-2</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2">
-        <f t="shared" si="0"/>
-        <v>2.0358599999999998E-2</v>
+        <f>AVERAGE(D8:H8)</f>
+        <v>1.7020799999999999E-2</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="1"/>
-        <v>1.9255000000000001E-2</v>
+        <f>MIN(D8:H8)</f>
+        <v>1.6709999999999999E-2</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="2">
-        <f>$M$6/4</f>
-        <v>2.7637500000000001E-3</v>
+        <f>$M$6/B8</f>
+        <v>6.3447499999999997E-3</v>
       </c>
       <c r="N8" s="3">
         <f>$K$6/K8</f>
-        <v>0.57413658789924693</v>
+        <v>1.5187911430281269</v>
       </c>
       <c r="O8" s="1">
         <v>4</v>
@@ -7555,43 +7747,45 @@
     <row r="9" spans="1:23">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2">
-        <v>2.3469E-2</v>
+        <v>2.0275999999999999E-2</v>
       </c>
       <c r="E9" s="2">
-        <v>2.3827000000000001E-2</v>
+        <v>1.9903000000000001E-2</v>
       </c>
       <c r="F9" s="2">
-        <v>2.4065E-2</v>
+        <v>2.2898999999999999E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>2.4671999999999999E-2</v>
+        <v>1.9255000000000001E-2</v>
       </c>
       <c r="H9" s="2">
-        <v>2.4181000000000001E-2</v>
+        <v>1.9460000000000002E-2</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="2">
-        <f t="shared" si="0"/>
-        <v>2.4042800000000003E-2</v>
+        <f>AVERAGE(D9:H9)</f>
+        <v>2.0358599999999998E-2</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="1"/>
-        <v>2.3469E-2</v>
+        <f>MIN(D9:H9)</f>
+        <v>1.9255000000000001E-2</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="2">
-        <f>$M$6/8</f>
-        <v>1.3818750000000001E-3</v>
+        <f>$M$6/B9</f>
+        <v>3.1723749999999998E-3</v>
       </c>
       <c r="N9" s="3">
         <f>$K$6/K9</f>
-        <v>0.47104691294899659</v>
-      </c>
-      <c r="O9" s="1"/>
+        <v>1.3180472604518305</v>
+      </c>
+      <c r="O9" s="1">
+        <v>8</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -7604,41 +7798,41 @@
     <row r="10" spans="1:23">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2">
-        <v>2.7639E-2</v>
+        <v>2.3469E-2</v>
       </c>
       <c r="E10" s="2">
-        <v>2.6969E-2</v>
+        <v>2.3827000000000001E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>2.8320000000000001E-2</v>
+        <v>2.4065E-2</v>
       </c>
       <c r="G10" s="2">
-        <v>2.6971999999999999E-2</v>
+        <v>2.4671999999999999E-2</v>
       </c>
       <c r="H10" s="2">
-        <v>2.7817000000000001E-2</v>
+        <v>2.4181000000000001E-2</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="2">
-        <f t="shared" si="0"/>
-        <v>2.7543400000000003E-2</v>
+        <f>AVERAGE(D10:H10)</f>
+        <v>2.4042800000000003E-2</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="1"/>
-        <v>2.6969E-2</v>
+        <f>MIN(D10:H10)</f>
+        <v>2.3469E-2</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="2">
-        <f>$M$6/12</f>
-        <v>9.2125000000000009E-4</v>
+        <f>$M$6/B10</f>
+        <v>1.5861874999999999E-3</v>
       </c>
       <c r="N10" s="3">
         <f>$K$6/K10</f>
-        <v>0.4099150876932775</v>
+        <v>1.081383953300098</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -7653,41 +7847,41 @@
     <row r="11" spans="1:23">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2">
-        <v>7.4031E-2</v>
+        <v>2.7639E-2</v>
       </c>
       <c r="E11" s="2">
-        <v>3.3123E-2</v>
+        <v>2.6969E-2</v>
       </c>
       <c r="F11" s="2">
-        <v>3.3031999999999999E-2</v>
+        <v>2.8320000000000001E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>3.4818000000000002E-2</v>
+        <v>2.6971999999999999E-2</v>
       </c>
       <c r="H11" s="2">
-        <v>4.4824000000000003E-2</v>
+        <v>2.7817000000000001E-2</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2">
-        <f t="shared" si="0"/>
-        <v>4.3965600000000001E-2</v>
+        <f>AVERAGE(D11:H11)</f>
+        <v>2.7543400000000003E-2</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="1"/>
-        <v>3.3031999999999999E-2</v>
+        <f>MIN(D11:H11)</f>
+        <v>2.6969E-2</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="2">
-        <f>$M$6/16</f>
-        <v>6.9093750000000004E-4</v>
+        <f>$M$6/B11</f>
+        <v>1.0574583333333332E-3</v>
       </c>
       <c r="N11" s="3">
         <f>$K$6/K11</f>
-        <v>0.33467546621457983</v>
+        <v>0.94104342022321918</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -7701,19 +7895,43 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="9">
+        <v>32</v>
+      </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="D12" s="2">
+        <v>7.4031E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3.3123E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3.3031999999999999E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3.4818000000000002E-2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4.4824000000000003E-2</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="J12" s="2">
+        <f>AVERAGE(D12:H12)</f>
+        <v>4.3965600000000001E-2</v>
+      </c>
+      <c r="K12" s="2">
+        <f>MIN(D12:H12)</f>
+        <v>3.3031999999999999E-2</v>
+      </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="M12" s="2">
+        <f>$M$6/B12</f>
+        <v>7.9309374999999996E-4</v>
+      </c>
+      <c r="N12" s="3">
+        <f>$K$6/K12</f>
+        <v>0.76831557277791229</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -8402,10 +8620,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:X11"/>
+  <dimension ref="B2:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8484,38 +8702,37 @@
     </row>
     <row r="5" spans="2:24" ht="8" customHeight="1"/>
     <row r="6" spans="2:24">
-      <c r="B6" s="9">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>191.695167</v>
-      </c>
-      <c r="E6" s="2">
-        <v>184.80751699999999</v>
-      </c>
-      <c r="F6" s="2">
-        <v>194.19979699999999</v>
-      </c>
-      <c r="G6" s="2">
-        <v>194.861458</v>
-      </c>
-      <c r="H6" s="2">
-        <v>217.36057500000001</v>
-      </c>
-      <c r="O6" s="2">
-        <f t="shared" ref="O6:O11" si="0">AVERAGE(D6:H6)</f>
-        <v>196.58490280000001</v>
-      </c>
-      <c r="P6" s="2">
-        <f t="shared" ref="P6:P11" si="1">MIN(D6:H6)</f>
-        <v>184.80751699999999</v>
-      </c>
-      <c r="R6" s="2">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>502.771478</v>
+      </c>
+      <c r="E6" s="1">
+        <v>507.14761800000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>485.35223400000001</v>
+      </c>
+      <c r="G6" s="1">
+        <v>500.96914299999997</v>
+      </c>
+      <c r="H6" s="1">
+        <v>480.461862</v>
+      </c>
+      <c r="O6" s="1">
+        <f>AVERAGE(D6:H6)</f>
+        <v>495.34046699999999</v>
+      </c>
+      <c r="P6" s="1">
+        <f>MIN(D6:H6)</f>
+        <v>480.461862</v>
+      </c>
+      <c r="R6" s="1">
         <f>P6</f>
-        <v>184.80751699999999</v>
-      </c>
-      <c r="S6" s="3">
-        <f>$P$6/P6</f>
+        <v>480.461862</v>
+      </c>
+      <c r="S6" s="1">
         <v>1</v>
       </c>
       <c r="T6" s="2">
@@ -8525,38 +8742,38 @@
     </row>
     <row r="7" spans="2:24">
       <c r="B7" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
-        <v>104.98876</v>
+        <v>191.695167</v>
       </c>
       <c r="E7" s="2">
-        <v>105.790733</v>
+        <v>184.80751699999999</v>
       </c>
       <c r="F7" s="2">
-        <v>102.57595600000001</v>
+        <v>194.19979699999999</v>
       </c>
       <c r="G7" s="2">
-        <v>104.64458</v>
+        <v>194.861458</v>
       </c>
       <c r="H7" s="2">
-        <v>119.727498</v>
+        <v>217.36057500000001</v>
       </c>
       <c r="O7" s="2">
-        <f t="shared" si="0"/>
-        <v>107.5455054</v>
+        <f>AVERAGE(D7:H7)</f>
+        <v>196.58490280000001</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" si="1"/>
-        <v>102.57595600000001</v>
+        <f>MIN(D7:H7)</f>
+        <v>184.80751699999999</v>
       </c>
       <c r="R7" s="2">
-        <f>$R$6/2</f>
-        <v>92.403758499999995</v>
+        <f>$R$6/B7</f>
+        <v>240.230931</v>
       </c>
       <c r="S7" s="3">
         <f>$P$6/P7</f>
-        <v>1.8016650705161352</v>
+        <v>2.5997961002852499</v>
       </c>
       <c r="T7" s="2">
         <f>2</f>
@@ -8565,38 +8782,38 @@
     </row>
     <row r="8" spans="2:24">
       <c r="B8" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>80.870994999999994</v>
+        <v>104.98876</v>
       </c>
       <c r="E8" s="2">
-        <v>80.141137999999998</v>
+        <v>105.790733</v>
       </c>
       <c r="F8" s="2">
-        <v>80.435023000000001</v>
+        <v>102.57595600000001</v>
       </c>
       <c r="G8" s="2">
-        <v>79.235023999999996</v>
+        <v>104.64458</v>
       </c>
       <c r="H8" s="2">
-        <v>84.942815999999993</v>
+        <v>119.727498</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" si="0"/>
-        <v>81.124999200000005</v>
+        <f>AVERAGE(D8:H8)</f>
+        <v>107.5455054</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" si="1"/>
-        <v>79.235023999999996</v>
+        <f>MIN(D8:H8)</f>
+        <v>102.57595600000001</v>
       </c>
       <c r="R8" s="2">
-        <f>$R$6/4</f>
-        <v>46.201879249999998</v>
+        <f>$R$6/B8</f>
+        <v>120.1154655</v>
       </c>
       <c r="S8" s="3">
         <f>$P$6/P8</f>
-        <v>2.3323968072502885</v>
+        <v>4.6839618243479979</v>
       </c>
       <c r="T8" s="2">
         <f>4</f>
@@ -8605,38 +8822,38 @@
     </row>
     <row r="9" spans="2:24">
       <c r="B9" s="9">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
-        <v>79.314853999999997</v>
+        <v>80.870994999999994</v>
       </c>
       <c r="E9" s="2">
-        <v>75.930788000000007</v>
+        <v>80.141137999999998</v>
       </c>
       <c r="F9" s="2">
-        <v>78.099710000000002</v>
+        <v>80.435023000000001</v>
       </c>
       <c r="G9" s="2">
-        <v>80.187123999999997</v>
+        <v>79.235023999999996</v>
       </c>
       <c r="H9" s="2">
-        <v>80.51764</v>
+        <v>84.942815999999993</v>
       </c>
       <c r="O9" s="2">
-        <f t="shared" si="0"/>
-        <v>78.810023200000003</v>
+        <f>AVERAGE(D9:H9)</f>
+        <v>81.124999200000005</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" si="1"/>
-        <v>75.930788000000007</v>
+        <f>MIN(D9:H9)</f>
+        <v>79.235023999999996</v>
       </c>
       <c r="R9" s="2">
-        <f>$R$6/8</f>
-        <v>23.100939624999999</v>
+        <f>$R$6/B9</f>
+        <v>60.05773275</v>
       </c>
       <c r="S9" s="3">
         <f>$P$6/P9</f>
-        <v>2.4338943644309339</v>
+        <v>6.0637561238070683</v>
       </c>
       <c r="T9" s="1">
         <v>8</v>
@@ -8644,74 +8861,110 @@
     </row>
     <row r="10" spans="2:24">
       <c r="B10" s="9">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2">
-        <v>88.001002</v>
+        <v>79.314853999999997</v>
       </c>
       <c r="E10" s="2">
-        <v>88.730462000000003</v>
+        <v>75.930788000000007</v>
       </c>
       <c r="F10" s="2">
-        <v>107.913887</v>
+        <v>78.099710000000002</v>
       </c>
       <c r="G10" s="2">
-        <v>126.60998600000001</v>
+        <v>80.187123999999997</v>
       </c>
       <c r="H10" s="2">
-        <v>104.670602</v>
+        <v>80.51764</v>
       </c>
       <c r="O10" s="2">
-        <f t="shared" si="0"/>
-        <v>103.18518779999999</v>
+        <f>AVERAGE(D10:H10)</f>
+        <v>78.810023200000003</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="1"/>
-        <v>88.001002</v>
+        <f>MIN(D10:H10)</f>
+        <v>75.930788000000007</v>
       </c>
       <c r="R10" s="2">
-        <f>$R$6/12</f>
-        <v>15.400626416666666</v>
+        <f>$R$6/B10</f>
+        <v>30.028866375</v>
       </c>
       <c r="S10" s="3">
         <f>$P$6/P10</f>
-        <v>2.1000615083905521</v>
+        <v>6.3276290771537882</v>
       </c>
     </row>
     <row r="11" spans="2:24">
       <c r="B11" s="9">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2">
-        <v>343.17010599999998</v>
+        <v>88.001002</v>
       </c>
       <c r="E11" s="2">
-        <v>308.16984600000001</v>
+        <v>88.730462000000003</v>
       </c>
       <c r="F11" s="2">
-        <v>321.52587599999998</v>
+        <v>107.913887</v>
       </c>
       <c r="G11" s="2">
-        <v>189.69341499999999</v>
+        <v>126.60998600000001</v>
       </c>
       <c r="H11" s="2">
-        <v>335.24965400000002</v>
+        <v>104.670602</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" si="0"/>
-        <v>299.56177939999998</v>
+        <f>AVERAGE(D11:H11)</f>
+        <v>103.18518779999999</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" si="1"/>
-        <v>189.69341499999999</v>
+        <f>MIN(D11:H11)</f>
+        <v>88.001002</v>
       </c>
       <c r="R11" s="2">
-        <f>$R$6/16</f>
-        <v>11.550469812499999</v>
+        <f>$R$6/B11</f>
+        <v>20.01924425</v>
       </c>
       <c r="S11" s="3">
         <f>$P$6/P11</f>
-        <v>0.97424318603784954</v>
+        <v>5.4597317198729165</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24">
+      <c r="B12" s="9">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2">
+        <v>343.17010599999998</v>
+      </c>
+      <c r="E12" s="2">
+        <v>308.16984600000001</v>
+      </c>
+      <c r="F12" s="2">
+        <v>321.52587599999998</v>
+      </c>
+      <c r="G12" s="2">
+        <v>189.69341499999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>335.24965400000002</v>
+      </c>
+      <c r="O12" s="2">
+        <f>AVERAGE(D12:H12)</f>
+        <v>299.56177939999998</v>
+      </c>
+      <c r="P12" s="2">
+        <f>MIN(D12:H12)</f>
+        <v>189.69341499999999</v>
+      </c>
+      <c r="R12" s="2">
+        <f>$R$6/B12</f>
+        <v>15.0144331875</v>
+      </c>
+      <c r="S12" s="3">
+        <f>$P$6/P12</f>
+        <v>2.5328336357906784</v>
       </c>
     </row>
   </sheetData>
@@ -8733,8 +8986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X38"/>
   <sheetViews>
-    <sheetView topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8849,24 +9102,23 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="1"/>
-      <c r="B6" s="9">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2">
-        <v>204.82372699999999</v>
-      </c>
-      <c r="E6" s="2">
-        <v>197.50738200000001</v>
-      </c>
-      <c r="F6" s="2">
-        <v>203.10920899999999</v>
-      </c>
-      <c r="G6" s="2">
-        <v>233.046932</v>
-      </c>
-      <c r="H6" s="2">
-        <v>198.07222999999999</v>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18">
+        <v>658.70205499999997</v>
+      </c>
+      <c r="E6" s="18">
+        <v>654.731764</v>
+      </c>
+      <c r="F6" s="18">
+        <v>657.87472000000002</v>
+      </c>
+      <c r="G6" s="18">
+        <v>650.32435499999997</v>
+      </c>
+      <c r="H6" s="18">
+        <v>649.43148499999995</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -8874,21 +9126,20 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="2">
-        <f t="shared" ref="O6:O11" si="0">AVERAGE(D6:H6)</f>
-        <v>207.31189599999999</v>
-      </c>
-      <c r="P6" s="2">
-        <f t="shared" ref="P6:P11" si="1">MIN(D6:H6)</f>
-        <v>197.50738200000001</v>
+      <c r="O6" s="18">
+        <f>AVERAGE(D6:H6)</f>
+        <v>654.21287580000001</v>
+      </c>
+      <c r="P6" s="18">
+        <f>MIN(D6:H6)</f>
+        <v>649.43148499999995</v>
       </c>
       <c r="Q6" s="1"/>
-      <c r="R6" s="2">
+      <c r="R6" s="18">
         <f>P6</f>
-        <v>197.50738200000001</v>
-      </c>
-      <c r="S6" s="3">
-        <f>1</f>
+        <v>649.43148499999995</v>
+      </c>
+      <c r="S6" s="18">
         <v>1</v>
       </c>
       <c r="T6" s="2">
@@ -8906,23 +9157,23 @@
     <row r="7" spans="1:24">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="2">
-        <v>93.552012000000005</v>
+        <v>204.82372699999999</v>
       </c>
       <c r="E7" s="2">
-        <v>110.451543</v>
+        <v>197.50738200000001</v>
       </c>
       <c r="F7" s="2">
-        <v>96.687968999999995</v>
+        <v>203.10920899999999</v>
       </c>
       <c r="G7" s="2">
-        <v>96.116731999999999</v>
+        <v>233.046932</v>
       </c>
       <c r="H7" s="2">
-        <v>103.198589</v>
+        <v>198.07222999999999</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -8931,21 +9182,21 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="2">
-        <f t="shared" si="0"/>
-        <v>100.001369</v>
+        <f>AVERAGE(D7:H7)</f>
+        <v>207.31189599999999</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" si="1"/>
-        <v>93.552012000000005</v>
+        <f>MIN(D7:H7)</f>
+        <v>197.50738200000001</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="2">
-        <f>$R$6/2</f>
-        <v>98.753691000000003</v>
+        <f>$R$6/B7</f>
+        <v>324.71574249999998</v>
       </c>
       <c r="S7" s="3">
         <f>$P$6/P7</f>
-        <v>2.1112040006151873</v>
+        <v>3.2881377821108475</v>
       </c>
       <c r="T7" s="2">
         <v>2</v>
@@ -8958,23 +9209,23 @@
     <row r="8" spans="1:24">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2">
-        <v>63.461308000000002</v>
+        <v>93.552012000000005</v>
       </c>
       <c r="E8" s="2">
-        <v>62.926752</v>
+        <v>110.451543</v>
       </c>
       <c r="F8" s="2">
-        <v>63.029746000000003</v>
+        <v>96.687968999999995</v>
       </c>
       <c r="G8" s="2">
-        <v>63.568255999999998</v>
+        <v>96.116731999999999</v>
       </c>
       <c r="H8" s="2">
-        <v>64.232428999999996</v>
+        <v>103.198589</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -8983,21 +9234,21 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="2">
-        <f t="shared" si="0"/>
-        <v>63.443698199999993</v>
+        <f>AVERAGE(D8:H8)</f>
+        <v>100.001369</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" si="1"/>
-        <v>62.926752</v>
+        <f>MIN(D8:H8)</f>
+        <v>93.552012000000005</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="2">
-        <f>$R$6/4</f>
-        <v>49.376845500000002</v>
+        <f>$R$6/B8</f>
+        <v>162.35787124999999</v>
       </c>
       <c r="S8" s="3">
         <f>$P$6/P8</f>
-        <v>3.1386870563413156</v>
+        <v>6.9419296401663697</v>
       </c>
       <c r="T8" s="2">
         <v>4</v>
@@ -9010,23 +9261,23 @@
     <row r="9" spans="1:24">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2">
-        <v>49.554572999999998</v>
+        <v>63.461308000000002</v>
       </c>
       <c r="E9" s="2">
-        <v>48.366109000000002</v>
+        <v>62.926752</v>
       </c>
       <c r="F9" s="2">
-        <v>50.200696000000001</v>
+        <v>63.029746000000003</v>
       </c>
       <c r="G9" s="2">
-        <v>50.805895</v>
+        <v>63.568255999999998</v>
       </c>
       <c r="H9" s="2">
-        <v>49.374671999999997</v>
+        <v>64.232428999999996</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -9035,21 +9286,21 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="2">
-        <f t="shared" si="0"/>
-        <v>49.660388999999995</v>
+        <f>AVERAGE(D9:H9)</f>
+        <v>63.443698199999993</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" si="1"/>
-        <v>48.366109000000002</v>
+        <f>MIN(D9:H9)</f>
+        <v>62.926752</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="2">
-        <f>$R$6/8</f>
-        <v>24.688422750000001</v>
+        <f>$R$6/B9</f>
+        <v>81.178935624999994</v>
       </c>
       <c r="S9" s="3">
         <f>$P$6/P9</f>
-        <v>4.0835904744787301</v>
+        <v>10.32043549617816</v>
       </c>
       <c r="T9" s="1">
         <v>8</v>
@@ -9062,23 +9313,23 @@
     <row r="10" spans="1:24">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2">
-        <v>45.371532000000002</v>
+        <v>49.554572999999998</v>
       </c>
       <c r="E10" s="2">
-        <v>46.038947</v>
+        <v>48.366109000000002</v>
       </c>
       <c r="F10" s="2">
-        <v>52.828918999999999</v>
+        <v>50.200696000000001</v>
       </c>
       <c r="G10" s="2">
-        <v>45.950128999999997</v>
+        <v>50.805895</v>
       </c>
       <c r="H10" s="2">
-        <v>46.894303000000001</v>
+        <v>49.374671999999997</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -9087,23 +9338,25 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="2">
-        <f t="shared" si="0"/>
-        <v>47.416766000000003</v>
+        <f>AVERAGE(D10:H10)</f>
+        <v>49.660388999999995</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="1"/>
-        <v>45.371532000000002</v>
+        <f>MIN(D10:H10)</f>
+        <v>48.366109000000002</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="2">
-        <f>$R$6/12</f>
-        <v>16.458948500000002</v>
+        <f>$R$6/B10</f>
+        <v>40.589467812499997</v>
       </c>
       <c r="S10" s="3">
         <f>$P$6/P10</f>
-        <v>4.3531124759022903</v>
-      </c>
-      <c r="T10" s="1"/>
+        <v>13.427408125801477</v>
+      </c>
+      <c r="T10" s="1">
+        <v>16</v>
+      </c>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
@@ -9112,23 +9365,23 @@
     <row r="11" spans="1:24">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2">
-        <v>65.632829000000001</v>
+        <v>45.371532000000002</v>
       </c>
       <c r="E11" s="2">
-        <v>62.674204000000003</v>
+        <v>46.038947</v>
       </c>
       <c r="F11" s="2">
-        <v>64.78537</v>
+        <v>52.828918999999999</v>
       </c>
       <c r="G11" s="2">
-        <v>70.718722999999997</v>
+        <v>45.950128999999997</v>
       </c>
       <c r="H11" s="2">
-        <v>70.842196999999999</v>
+        <v>46.894303000000001</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -9137,21 +9390,21 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="2">
-        <f t="shared" si="0"/>
-        <v>66.9306646</v>
+        <f>AVERAGE(D11:H11)</f>
+        <v>47.416766000000003</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" si="1"/>
-        <v>62.674204000000003</v>
+        <f>MIN(D11:H11)</f>
+        <v>45.371532000000002</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="2">
-        <f>$R$6/16</f>
-        <v>12.344211375</v>
+        <f>$R$6/B11</f>
+        <v>27.059645208333333</v>
       </c>
       <c r="S11" s="3">
         <f>$P$6/P11</f>
-        <v>3.1513345107661839</v>
+        <v>14.313633601792418</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -9161,24 +9414,48 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="9">
+        <v>32</v>
+      </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="D12" s="2">
+        <v>65.632829000000001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>62.674204000000003</v>
+      </c>
+      <c r="F12" s="2">
+        <v>64.78537</v>
+      </c>
+      <c r="G12" s="2">
+        <v>70.718722999999997</v>
+      </c>
+      <c r="H12" s="2">
+        <v>70.842196999999999</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="O12" s="2">
+        <f>AVERAGE(D12:H12)</f>
+        <v>66.9306646</v>
+      </c>
+      <c r="P12" s="2">
+        <f>MIN(D12:H12)</f>
+        <v>62.674204000000003</v>
+      </c>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
+      <c r="R12" s="2">
+        <f>$R$6/B12</f>
+        <v>20.294733906249999</v>
+      </c>
+      <c r="S12" s="3">
+        <f>$P$6/P12</f>
+        <v>10.362022068920092</v>
+      </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>

</xml_diff>